<commit_message>
Versão 0.3 PPJ e Versão 1.0 de PBL
</commit_message>
<xml_diff>
--- a/01-SISTEMA/01-REQUISITOS/PBL-Product Backlog.xlsx
+++ b/01-SISTEMA/01-REQUISITOS/PBL-Product Backlog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8235" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8235"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
   <si>
     <t>Nome / Descrição</t>
   </si>
@@ -52,14 +52,107 @@
     <t>Horas Trabalhadas</t>
   </si>
   <si>
-    <t>As colunas de E-H devem ser preenchidas quando um item de backlog for designado a uma iteração</t>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Alta</t>
+  </si>
+  <si>
+    <t>Manter funcionários setor administrativo</t>
+  </si>
+  <si>
+    <t>Média</t>
+  </si>
+  <si>
+    <t>Manter alunos</t>
+  </si>
+  <si>
+    <t>Manter assistentes sociais</t>
+  </si>
+  <si>
+    <t>Validar notas, frequência e matricula.</t>
+  </si>
+  <si>
+    <t>Manter editais de auxílios</t>
+  </si>
+  <si>
+    <t>Manter editais de doação</t>
+  </si>
+  <si>
+    <t>Baixa</t>
+  </si>
+  <si>
+    <t>Apresentar aos alunos editais abertos</t>
+  </si>
+  <si>
+    <t>Impedir inscrições de alunos com requisitos inválidos</t>
+  </si>
+  <si>
+    <t>Apresentar o Questionário Socioeconômico ao aluno</t>
+  </si>
+  <si>
+    <t>Inclusão de documentos no momento da inscrição</t>
+  </si>
+  <si>
+    <t>Gerenciamento de notificações para a assistente social</t>
+  </si>
+  <si>
+    <t>Pré-classificação dos alunos</t>
+  </si>
+  <si>
+    <t>Manter entrevistas</t>
+  </si>
+  <si>
+    <t>Manter vistas domiciliares</t>
+  </si>
+  <si>
+    <t>Divulgação automática dos resultados dos auxílios</t>
+  </si>
+  <si>
+    <t>Gerenciar Classificação final em editais</t>
+  </si>
+  <si>
+    <t>Validação de auxílio com termo de compromisso</t>
+  </si>
+  <si>
+    <t>Manter auxílios</t>
+  </si>
+  <si>
+    <t>Gerenciar materiais de doação</t>
+  </si>
+  <si>
+    <t>Manter doações feitas para alunos</t>
+  </si>
+  <si>
+    <t>Gerenciamento de notificações para o aluno</t>
+  </si>
+  <si>
+    <t>Listar alunos que receberam o pagamento do auxílio</t>
+  </si>
+  <si>
+    <t>Gerar relatório orçamental</t>
+  </si>
+  <si>
+    <t>Gerar relatório individual do aluno</t>
+  </si>
+  <si>
+    <t>Impressão de relatórios</t>
+  </si>
+  <si>
+    <t>Gerar relatório global dos alunos</t>
+  </si>
+  <si>
+    <t>PRODUCT BACKLOG</t>
+  </si>
+  <si>
+    <t>Suspensão automática de um auxílio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,12 +167,21 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -95,6 +197,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="41"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -126,15 +234,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -416,58 +530,589 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47" customWidth="1"/>
+    <col min="1" max="1" width="50.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" customWidth="1"/>
     <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" customWidth="1"/>
     <col min="7" max="7" width="9.85546875" customWidth="1"/>
     <col min="8" max="8" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="39" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+    </row>
+    <row r="2" spans="1:10" ht="39" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+      <c r="B3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="4">
+        <v>5</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="J3" s="7"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="4">
+        <v>2</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="J4" s="7"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="4">
+        <v>3</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="J5" s="7"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="4">
+        <v>2</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="J6" s="7"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="4">
+        <v>20</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="J7" s="7"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="4">
+        <v>5</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="J8" s="7"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="4">
+        <v>5</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="J9" s="7"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="4">
+        <v>3</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="J10" s="7"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="4">
+        <v>5</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="J11" s="7"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="4">
+        <v>3</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="J12" s="7"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="4">
+        <v>3</v>
+      </c>
+      <c r="D13" s="6">
+        <v>0</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="J13" s="7"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="4">
+        <v>5</v>
+      </c>
+      <c r="D14" s="6">
+        <v>0</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="J14" s="7"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="4">
+        <v>40</v>
+      </c>
+      <c r="D15" s="6">
+        <v>0</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="J15" s="7"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="4">
+        <v>13</v>
+      </c>
+      <c r="D16" s="6">
+        <v>0</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="J16" s="7"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="4">
+        <v>8</v>
+      </c>
+      <c r="D17" s="6">
+        <v>0</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="J17" s="7"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="4">
+        <v>5</v>
+      </c>
+      <c r="D18" s="6">
+        <v>0</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="J18" s="7"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="4">
+        <v>8</v>
+      </c>
+      <c r="D19" s="6">
+        <v>0</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="J19" s="7"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="4">
+        <v>3</v>
+      </c>
+      <c r="D20" s="6">
+        <v>0</v>
+      </c>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="J20" s="7"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="4">
+        <v>13</v>
+      </c>
+      <c r="D21" s="6">
+        <v>0</v>
+      </c>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="4">
+        <v>8</v>
+      </c>
+      <c r="D22" s="6">
+        <v>0</v>
+      </c>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="4">
+        <v>5</v>
+      </c>
+      <c r="D23" s="6">
+        <v>0</v>
+      </c>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="4">
+        <v>2</v>
+      </c>
+      <c r="D24" s="6">
+        <v>0</v>
+      </c>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="4">
+        <v>5</v>
+      </c>
+      <c r="D25" s="6">
+        <v>0</v>
+      </c>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="4">
+        <v>3</v>
+      </c>
+      <c r="D26" s="6">
+        <v>0</v>
+      </c>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="4">
+        <v>3</v>
+      </c>
+      <c r="D27" s="6">
+        <v>0</v>
+      </c>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="4">
+        <v>3</v>
+      </c>
+      <c r="D28" s="6">
+        <v>0</v>
+      </c>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="4">
+        <v>2</v>
+      </c>
+      <c r="D29" s="6">
+        <v>0</v>
+      </c>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="4">
+        <v>3</v>
+      </c>
+      <c r="D30" s="6">
+        <v>0</v>
+      </c>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -487,7 +1132,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>